<commit_message>
Added a marking sheet spreadsheet
</commit_message>
<xml_diff>
--- a/MarkingSheet/marking-sheet.xlsx
+++ b/MarkingSheet/marking-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\SEM_group_project\MarkingSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D3045ED-A3EF-43B5-90B1-C902B9D02AF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA1648F-5E0F-4AEA-84FA-6B16C8697CDC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9918A3FF-DBD3-4DC8-955A-713BDC2EB953}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +117,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,13 +146,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,7 +475,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,8 +488,8 @@
     <col min="6" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3"/>

</xml_diff>